<commit_message>
Updated username to admin
</commit_message>
<xml_diff>
--- a/selenium/com.ChildWelfareAutomationSuite.POC/ApplicationTestData/AppData.xlsx
+++ b/selenium/com.ChildWelfareAutomationSuite.POC/ApplicationTestData/AppData.xlsx
@@ -16,24 +16,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Sravan.neppalli@cgi.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>admin@cgi.com</t>
+  </si>
+  <si>
+    <t>adminpw</t>
+  </si>
+  <si>
+    <t>AdminUsername</t>
+  </si>
+  <si>
+    <t>AdminPassword</t>
+  </si>
+  <si>
+    <t>StandardUser</t>
+  </si>
+  <si>
+    <t>StandardPassword</t>
+  </si>
+  <si>
+    <t>sravan.neppalli@cgi.com</t>
   </si>
   <si>
     <t>ddff444</t>
   </si>
   <si>
-    <t>ErrorMesg</t>
-  </si>
-  <si>
-    <t>SucessMesg</t>
+    <t>NonRegisterUser</t>
+  </si>
+  <si>
+    <t>venkat@cgi.com</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>venkat</t>
   </si>
 </sst>
 </file>
@@ -391,26 +409,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -418,18 +438,38 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>